<commit_message>
campo origemRecurso - geracao txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OliveiD1\Desktop\SS84832\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbinth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="184">
   <si>
     <t>CAMPO</t>
   </si>
@@ -572,14 +572,55 @@
     <t>Formato 0000000000000000,00</t>
   </si>
   <si>
-    <t>Pode ser Negativo. Formato 00000000000000,00</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pode ser Negativo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Formato 00000000000000,00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Pode ser Negativo. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Formato 00000000000000,00</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,8 +649,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +679,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -737,6 +797,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -749,6 +810,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1031,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,14 +1109,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1115,14 +1179,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1383,7 +1447,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1403,7 +1467,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1421,7 +1485,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="24" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1439,7 +1503,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1455,11 +1519,11 @@
         <v>138</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1477,7 +1541,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1495,7 +1559,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1948,7 +2012,7 @@
       <c r="E51" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="20" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1968,7 +2032,7 @@
       <c r="E52" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="F52" s="20"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
@@ -1986,7 +2050,7 @@
       <c r="E53" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="F53" s="21"/>
+      <c r="F53" s="22"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
@@ -1997,14 +2061,14 @@
       <c r="F54" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2209,14 +2273,14 @@
       <c r="F67" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2297,14 +2361,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">

</xml_diff>

<commit_message>
campo grupoHabitacional - geracao txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1559,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1577,7 +1577,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1595,7 +1595,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1613,7 +1613,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1631,7 +1631,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="5" t="s">

</xml_diff>

<commit_message>
campo produtoFinanceiro - geracao txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -1095,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1649,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="5" t="s">

</xml_diff>

<commit_message>
campo telCelular - gravar txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="185">
   <si>
     <t>CAMPO</t>
   </si>
@@ -347,12 +347,6 @@
     <t>220</t>
   </si>
   <si>
-    <t>326</t>
-  </si>
-  <si>
-    <t>327</t>
-  </si>
-  <si>
     <t>TIPO REGISTRO SITUAÇÃO ESPECIAL</t>
   </si>
   <si>
@@ -428,9 +422,6 @@
     <t>Esses campos serão preenchidos se no atendimento for identificado telefone e e-mail alternativo de contato que não foi cadastrado para o contrato.</t>
   </si>
   <si>
-    <t>476</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
@@ -513,60 +504,6 @@
   </si>
   <si>
     <t>273</t>
-  </si>
-  <si>
-    <t>276</t>
-  </si>
-  <si>
-    <t>277</t>
-  </si>
-  <si>
-    <t>287</t>
-  </si>
-  <si>
-    <t>288</t>
-  </si>
-  <si>
-    <t>301</t>
-  </si>
-  <si>
-    <t>302</t>
-  </si>
-  <si>
-    <t>328</t>
-  </si>
-  <si>
-    <t>329</t>
-  </si>
-  <si>
-    <t>336</t>
-  </si>
-  <si>
-    <t>337</t>
-  </si>
-  <si>
-    <t>396</t>
-  </si>
-  <si>
-    <t>397</t>
-  </si>
-  <si>
-    <t>414</t>
-  </si>
-  <si>
-    <t>415</t>
-  </si>
-  <si>
-    <t>475</t>
-  </si>
-  <si>
-    <t>479</t>
-  </si>
-  <si>
-    <t>480</t>
-  </si>
-  <si>
-    <t>488</t>
   </si>
   <si>
     <t>Formato 0000000000000000,00</t>
@@ -614,6 +551,72 @@
       </rPr>
       <t>Formato 00000000000000,00</t>
     </r>
+  </si>
+  <si>
+    <t>276 /277</t>
+  </si>
+  <si>
+    <t>4 --&gt; 5</t>
+  </si>
+  <si>
+    <t>277 / 278</t>
+  </si>
+  <si>
+    <t>287 /288</t>
+  </si>
+  <si>
+    <t>288 / 289</t>
+  </si>
+  <si>
+    <t>301 / 302</t>
+  </si>
+  <si>
+    <t>302 / 303</t>
+  </si>
+  <si>
+    <t>326 / 327</t>
+  </si>
+  <si>
+    <t>327 / 328</t>
+  </si>
+  <si>
+    <t>328 / 329</t>
+  </si>
+  <si>
+    <t>329 / 330</t>
+  </si>
+  <si>
+    <t>336 / 337</t>
+  </si>
+  <si>
+    <t>337 / 338</t>
+  </si>
+  <si>
+    <t>396 / 397</t>
+  </si>
+  <si>
+    <t>397 / 398</t>
+  </si>
+  <si>
+    <t>414 / 416</t>
+  </si>
+  <si>
+    <t>415 / 417</t>
+  </si>
+  <si>
+    <t>475 / 477</t>
+  </si>
+  <si>
+    <t>476 / 478</t>
+  </si>
+  <si>
+    <t>479 / 481</t>
+  </si>
+  <si>
+    <t>480 / 482</t>
+  </si>
+  <si>
+    <t>488 / 490</t>
   </si>
 </sst>
 </file>
@@ -768,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -798,6 +801,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,9 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,14 +1113,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1139,7 +1143,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1159,7 +1163,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1175,18 +1179,18 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1209,7 +1213,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1229,7 +1233,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1247,7 +1251,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1265,7 +1269,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1283,7 +1287,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1301,7 +1305,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1319,7 +1323,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1337,7 +1341,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1355,7 +1359,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1373,7 +1377,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1391,7 +1395,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1409,7 +1413,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1427,7 +1431,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1463,11 +1467,11 @@
         <v>94</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1477,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>95</v>
@@ -1485,7 +1489,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1495,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>96</v>
@@ -1503,7 +1507,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1513,17 +1517,17 @@
         <v>52</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1533,15 +1537,15 @@
         <v>4</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="19" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1554,12 +1558,12 @@
         <v>97</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1572,12 +1576,12 @@
         <v>98</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1590,12 +1594,12 @@
         <v>99</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1605,7 +1609,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>100</v>
@@ -1613,7 +1617,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1623,15 +1627,15 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1641,15 +1645,15 @@
         <v>5</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1659,33 +1663,33 @@
         <v>4</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="4">
-        <v>4</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1695,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>101</v>
@@ -1703,7 +1707,7 @@
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1716,14 +1720,14 @@
         <v>102</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1733,17 +1737,17 @@
         <v>8</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1753,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>103</v>
@@ -1761,7 +1765,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="19" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1779,7 +1783,7 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1789,15 +1793,15 @@
         <v>1</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1810,12 +1814,12 @@
         <v>105</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="19" t="s">
         <v>74</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1828,12 +1832,12 @@
         <v>106</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1843,25 +1847,25 @@
         <v>50</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="19" t="s">
         <v>76</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="4">
-        <v>4</v>
+      <c r="C43" s="26" t="s">
+        <v>164</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>163</v>
@@ -1869,7 +1873,7 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1879,15 +1883,15 @@
         <v>11</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -1897,15 +1901,15 @@
         <v>14</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1915,15 +1919,15 @@
         <v>25</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -1933,15 +1937,15 @@
         <v>2</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>108</v>
+        <v>171</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="19" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -1951,15 +1955,15 @@
         <v>8</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1969,15 +1973,15 @@
         <v>60</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -1987,18 +1991,18 @@
         <v>84</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>9</v>
@@ -2007,18 +2011,18 @@
         <v>60</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>133</v>
+        <v>180</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>11</v>
@@ -2027,16 +2031,16 @@
         <v>4</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="F52" s="21"/>
+        <v>182</v>
+      </c>
+      <c r="F52" s="24"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>11</v>
@@ -2045,12 +2049,12 @@
         <v>9</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F53" s="22"/>
+        <v>184</v>
+      </c>
+      <c r="F53" s="25"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
@@ -2061,14 +2065,14 @@
       <c r="F54" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2091,7 +2095,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2111,7 +2115,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2129,7 +2133,7 @@
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="19" t="s">
         <v>42</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -2147,7 +2151,7 @@
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -2165,8 +2169,8 @@
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>119</v>
+      <c r="A62" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>11</v>
@@ -2183,8 +2187,8 @@
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>120</v>
+      <c r="A63" s="20" t="s">
+        <v>118</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>11</v>
@@ -2201,8 +2205,8 @@
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>121</v>
+      <c r="A64" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="B64" s="15" t="s">
         <v>11</v>
@@ -2214,13 +2218,13 @@
         <v>30</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>122</v>
+      <c r="A65" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="B65" s="15" t="s">
         <v>11</v>
@@ -2232,13 +2236,13 @@
         <v>31</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>123</v>
+      <c r="A66" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="B66" s="15" t="s">
         <v>11</v>
@@ -2250,13 +2254,13 @@
         <v>41</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F66" s="14"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
-        <v>124</v>
+      <c r="A67" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>11</v>
@@ -2265,22 +2269,22 @@
         <v>9</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F67" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
+      <c r="A69" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2303,7 +2307,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2319,11 +2323,11 @@
         <v>10</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B72" s="5" t="s">
@@ -2341,8 +2345,8 @@
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>111</v>
+      <c r="A73" s="19" t="s">
+        <v>109</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>11</v>
@@ -2354,21 +2358,21 @@
         <v>35</v>
       </c>
       <c r="E73" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="F73" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2407,7 +2411,7 @@
         <v>10</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,7 +2434,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>11</v>
@@ -2442,10 +2446,10 @@
         <v>35</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
campo telAlternativo - gravar txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -607,16 +607,16 @@
     <t>475 / 477</t>
   </si>
   <si>
-    <t>476 / 478</t>
-  </si>
-  <si>
-    <t>479 / 481</t>
-  </si>
-  <si>
-    <t>480 / 482</t>
-  </si>
-  <si>
-    <t>488 / 490</t>
+    <t>476 / 477</t>
+  </si>
+  <si>
+    <t>479 / 480</t>
+  </si>
+  <si>
+    <t>480 / 481</t>
+  </si>
+  <si>
+    <t>488 / 489</t>
   </si>
 </sst>
 </file>
@@ -804,6 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -816,7 +817,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,14 +1113,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1183,14 +1183,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1861,7 +1861,7 @@
       <c r="B43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="22" t="s">
         <v>164</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2001,7 +2001,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B51" s="15" t="s">
@@ -2016,12 +2016,12 @@
       <c r="E51" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="24" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="19" t="s">
         <v>128</v>
       </c>
       <c r="B52" s="15" t="s">
@@ -2036,10 +2036,10 @@
       <c r="E52" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="25"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -2054,7 +2054,7 @@
       <c r="E53" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="F53" s="25"/>
+      <c r="F53" s="26"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
@@ -2065,14 +2065,14 @@
       <c r="F54" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2277,14 +2277,14 @@
       <c r="F67" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2365,14 +2365,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2395,7 +2395,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -2415,7 +2415,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2433,7 +2433,7 @@
       <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B79" s="8" t="s">

</xml_diff>

<commit_message>
correcao campo ValorDivida - gravar negativo txt
</commit_message>
<xml_diff>
--- a/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
+++ b/novo_layout_CAIXA_por_tipo_registro_v5.xlsx
@@ -604,9 +604,6 @@
     <t>415 / 417</t>
   </si>
   <si>
-    <t>475 / 477</t>
-  </si>
-  <si>
     <t>476 / 477</t>
   </si>
   <si>
@@ -617,6 +614,9 @@
   </si>
   <si>
     <t>488 / 489</t>
+  </si>
+  <si>
+    <t>475 / 476</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,12 +682,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -801,8 +795,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1099,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,14 +1105,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1143,7 +1135,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1163,7 +1155,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1183,14 +1175,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1213,7 +1205,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1233,7 +1225,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1251,7 +1243,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1269,7 +1261,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1287,7 +1279,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1305,7 +1297,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1323,7 +1315,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1341,7 +1333,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1359,7 +1351,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1377,7 +1369,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1395,7 +1387,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1413,7 +1405,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1431,7 +1423,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1471,7 +1463,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1489,7 +1481,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1507,7 +1499,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="19" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1527,7 +1519,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1545,7 +1537,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1563,7 +1555,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1581,7 +1573,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1599,7 +1591,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1617,7 +1609,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1635,7 +1627,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1653,7 +1645,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="18" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1671,7 +1663,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -1689,7 +1681,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1707,7 +1699,7 @@
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1727,7 +1719,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="18" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1747,7 +1739,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1765,7 +1757,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1783,7 +1775,7 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1801,7 +1793,7 @@
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="18" t="s">
         <v>73</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1819,7 +1811,7 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>74</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1837,7 +1829,7 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>75</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1855,13 +1847,13 @@
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>76</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="20" t="s">
         <v>164</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -1873,7 +1865,7 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1891,7 +1883,7 @@
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -1909,7 +1901,7 @@
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="18" t="s">
         <v>79</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1927,7 +1919,7 @@
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>80</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -1945,7 +1937,7 @@
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -1963,7 +1955,7 @@
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1981,7 +1973,7 @@
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -2001,7 +1993,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="18" t="s">
         <v>130</v>
       </c>
       <c r="B51" s="15" t="s">
@@ -2014,14 +2006,14 @@
         <v>179</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="F51" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F51" s="22" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="18" t="s">
         <v>128</v>
       </c>
       <c r="B52" s="15" t="s">
@@ -2031,15 +2023,15 @@
         <v>4</v>
       </c>
       <c r="D52" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E52" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="F52" s="25"/>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="18" t="s">
         <v>129</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -2049,12 +2041,12 @@
         <v>9</v>
       </c>
       <c r="D53" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="F53" s="26"/>
+      <c r="F53" s="24"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
@@ -2065,14 +2057,14 @@
       <c r="F54" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2095,7 +2087,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2115,7 +2107,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2133,7 +2125,7 @@
       <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -2151,7 +2143,7 @@
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -2169,7 +2161,7 @@
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="18" t="s">
         <v>117</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -2187,7 +2179,7 @@
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="19" t="s">
         <v>118</v>
       </c>
       <c r="B63" s="8" t="s">
@@ -2205,7 +2197,7 @@
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="18" t="s">
         <v>119</v>
       </c>
       <c r="B64" s="15" t="s">
@@ -2223,7 +2215,7 @@
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="19" t="s">
         <v>120</v>
       </c>
       <c r="B65" s="15" t="s">
@@ -2241,7 +2233,7 @@
       <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="18" t="s">
         <v>121</v>
       </c>
       <c r="B66" s="15" t="s">
@@ -2259,7 +2251,7 @@
       <c r="F66" s="14"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="19" t="s">
         <v>122</v>
       </c>
       <c r="B67" s="15" t="s">
@@ -2277,14 +2269,14 @@
       <c r="F67" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2307,7 +2299,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2327,7 +2319,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B72" s="5" t="s">
@@ -2345,7 +2337,7 @@
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="18" t="s">
         <v>109</v>
       </c>
       <c r="B73" s="8" t="s">
@@ -2365,14 +2357,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2395,7 +2387,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -2415,7 +2407,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2433,7 +2425,7 @@
       <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="18" t="s">
         <v>115</v>
       </c>
       <c r="B79" s="8" t="s">

</xml_diff>